<commit_message>
Refactoring und Tests angepasst
</commit_message>
<xml_diff>
--- a/test_data/testCreateBMEcatFromExcelFullDataFiege.xlsx
+++ b/test_data/testCreateBMEcatFromExcelFullDataFiege.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="92">
   <si>
     <t>articleType</t>
   </si>
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AW3" sqref="AW3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,8 +825,8 @@
       <c r="H2" t="s">
         <v>57</v>
       </c>
-      <c r="I2" t="s">
-        <v>58</v>
+      <c r="I2">
+        <v>1.5</v>
       </c>
       <c r="J2" t="s">
         <v>59</v>

</xml_diff>